<commit_message>
written part of the report
</commit_message>
<xml_diff>
--- a/Code/Different sensor weights test.xlsx
+++ b/Code/Different sensor weights test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School Stuff\2001 Systems Design\QuadCopter\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCB11BF5-41D9-43A5-B3DE-CA2D6F3EBFB5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2" xr2:uid="{EE705B06-9F18-4725-A642-D4FC1264A143}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" xr2:uid="{EE705B06-9F18-4725-A642-D4FC1264A143}"/>
   </bookViews>
   <sheets>
     <sheet name="w=15" sheetId="3" r:id="rId1"/>
@@ -22,7 +23,7 @@
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">'w=25'!$A$1:$D$403</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'w=30'!$A$1:$D$332</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,23 +34,23 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{7AB9EF9A-0603-4EBA-88A3-A7D13FC2CFCA}" keepAlive="1" name="Query - DATALOG" description="Connection to the 'DATALOG' query in the workbook." type="5" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Query - DATALOG" description="Connection to the 'DATALOG' query in the workbook." type="5" refreshedVersion="0" background="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=DATALOG;Extended Properties=&quot;&quot;" command="SELECT * FROM [DATALOG]"/>
   </connection>
-  <connection id="2" xr16:uid="{A03B6CB8-15E0-4817-A672-F6F96AA0A581}" keepAlive="1" name="Query - DATALOG (2)" description="Connection to the 'DATALOG (2)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Query - DATALOG (2)" description="Connection to the 'DATALOG (2)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=DATALOG (2);Extended Properties=&quot;&quot;" command="SELECT * FROM [DATALOG (2)]"/>
   </connection>
-  <connection id="3" xr16:uid="{4609C64B-760B-4C9D-BCA4-E31903D120FD}" keepAlive="1" name="Query - DATALOG (3)" description="Connection to the 'DATALOG (3)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" keepAlive="1" name="Query - DATALOG (3)" description="Connection to the 'DATALOG (3)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=DATALOG (3);Extended Properties=&quot;&quot;" command="SELECT * FROM [DATALOG (3)]"/>
   </connection>
-  <connection id="4" xr16:uid="{1C745BF4-2B7B-4D38-892E-7984197BE14F}" keepAlive="1" name="Query - DATALOG (4)" description="Connection to the 'DATALOG (4)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" keepAlive="1" name="Query - DATALOG (4)" description="Connection to the 'DATALOG (4)' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=DATALOG (4);Extended Properties=&quot;&quot;" command="SELECT * FROM [DATALOG (4)]"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Column1</t>
   </si>
@@ -64,6 +65,15 @@
   </si>
   <si>
     <t>delay 86</t>
+  </si>
+  <si>
+    <t>Altitude reading</t>
+  </si>
+  <si>
+    <t>Smoothened altitude</t>
+  </si>
+  <si>
+    <t>Actual altitude</t>
   </si>
 </sst>
 </file>
@@ -177,7 +187,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column2</c:v>
+                  <c:v>Actual altitude</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2004,7 +2014,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column3</c:v>
+                  <c:v>Smoothened altitude</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3837,6 +3847,8 @@
         <c:axId val="1703799311"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="15000"/>
+          <c:min val="10000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4099,7 +4111,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column2</c:v>
+                  <c:v>Altitude reading</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6136,7 +6148,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Column3</c:v>
+                  <c:v>Smoothened altitude</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8179,6 +8191,8 @@
         <c:axId val="1727754767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="34000"/>
+          <c:min val="22000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -8196,6 +8210,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -8258,6 +8327,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Altitude</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (cm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -15289,16 +15418,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>476251</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514352</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15368,7 +15497,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{C803A830-9BD6-4923-9E1D-676132CE5CEF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -15381,7 +15510,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="3" xr16:uid="{21B402CC-1E55-44AA-A841-C624D91DBF46}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -15394,7 +15523,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{4D934C5D-D618-4509-A7DB-782E8DF2A4CB}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="4" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="5">
     <queryTableFields count="4">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -15411,8 +15540,8 @@
   <autoFilter ref="A1:D297" xr:uid="{8740BC7C-E38E-4351-815E-70CEB2E32828}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3BBF946F-C060-4951-A057-241A11956EDD}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{DEE9DF08-F0A9-49BF-9921-561371468DB3}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{08074CF8-13E3-4BB7-B2BF-A55F4FFBA560}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
+    <tableColumn id="2" xr3:uid="{DEE9DF08-F0A9-49BF-9921-561371468DB3}" uniqueName="2" name="Actual altitude" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{08074CF8-13E3-4BB7-B2BF-A55F4FFBA560}" uniqueName="3" name="Smoothened altitude" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{1DB3A9AB-0CC4-4551-BA1F-3E918A687C7F}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15424,8 +15553,8 @@
   <autoFilter ref="A1:D332" xr:uid="{DA2C7546-FFF0-4690-AB80-62AB6DB23702}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F59F0B04-2781-4EC0-9D08-F687EF7A8082}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{F186DDD4-87D8-4D27-9115-4A4771FD76AC}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{9F1FB68E-8D33-4015-91AC-1925704E8C82}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
+    <tableColumn id="2" xr3:uid="{F186DDD4-87D8-4D27-9115-4A4771FD76AC}" uniqueName="2" name="Altitude reading" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{9F1FB68E-8D33-4015-91AC-1925704E8C82}" uniqueName="3" name="Smoothened altitude" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{624B365C-1567-4102-87C2-D9746237ADA1}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -15745,8 +15874,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F297"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15759,10 +15888,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -19929,8 +20058,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D332"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="F5" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19943,10 +20072,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -24600,7 +24729,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D403"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>